<commit_message>
Added 25x4 more manual investigation of individual tool's results
</commit_message>
<xml_diff>
--- a/manual/simian_default_combined.xlsx
+++ b/manual/simian_default_combined.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="6380" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="simian_default_combined" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="171">
   <si>
     <t>stackoverflow_formatted/92962_0.java</t>
   </si>
@@ -458,9 +458,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -489,6 +486,60 @@
   </si>
   <si>
     <t>SO answer says that the code is copied from BasicAuthenticator from Tomcat project. There might be some relationships.</t>
+  </si>
+  <si>
+    <t>SO answer says that the code is copied from Hibernate's ConnectionProviderInitiator.java</t>
+  </si>
+  <si>
+    <t>SO answer says that the code is copied and modified from Hadoop wordcount example.</t>
+  </si>
+  <si>
+    <t>duplicate with ok pairs</t>
+  </si>
+  <si>
+    <t>duplicate with other pairs with the same Qualitas file investigated before</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>getter and setter which are accidentally similar</t>
+  </si>
+  <si>
+    <t>SO answer says that the code is an exact copy from JRVerifier.java</t>
+  </si>
+  <si>
+    <t>boiler-plate code of creating a socket connection</t>
+  </si>
+  <si>
+    <t>SO answer says that the code is copied and modified from Hadoop DbCountPageView example.</t>
+  </si>
+  <si>
+    <t>SO answer says that the code is copied from JUnit assertEquals()</t>
+  </si>
+  <si>
+    <t>SO answer says that the code is copied and modified from Hadoop org.hibernate.criterion.Example example.</t>
+  </si>
+  <si>
+    <t>SO answer says that the code is copied from JUnit ExternalResource</t>
+  </si>
+  <si>
+    <t>SO answer says that the code is copied from a book called Filthy Rich Clients (http://filthyrichclients.org). iReport code doesn't say anything about copying.</t>
+  </si>
+  <si>
+    <t>SO answer shows a code that extends from SpiderWebPlot in JFreeChart.</t>
+  </si>
+  <si>
+    <t>SO answer mentions that the code there is an investigation of code in getProcessedSql() in Hibernate.</t>
+  </si>
+  <si>
+    <t>SO answer says that it copies the code from ExpectException.java ("an exxcerpt from the Junit source code (ExpectException.java):")</t>
+  </si>
+  <si>
+    <t>both have exactly similar hashCode() and equals() methods.</t>
+  </si>
+  <si>
+    <t>both have very similar implementation of checking certificate of SSL connection.</t>
   </si>
 </sst>
 </file>
@@ -803,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L94"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,7 +865,7 @@
     <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84.33203125" customWidth="1"/>
+    <col min="5" max="5" width="123.83203125" customWidth="1"/>
     <col min="6" max="7" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -823,307 +874,271 @@
     <col min="12" max="12" width="69.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="B1">
+        <v>77</v>
+      </c>
+      <c r="C1">
+        <v>134</v>
+      </c>
+      <c r="D1">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1">
+        <v>85</v>
+      </c>
+      <c r="G1">
+        <v>142</v>
+      </c>
+      <c r="H1">
+        <v>58</v>
+      </c>
+      <c r="I1">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="F2">
+        <v>82</v>
+      </c>
+      <c r="G2">
+        <v>131</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <v>57</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="D1">
+      <c r="F4">
+        <v>81</v>
+      </c>
+      <c r="G4">
+        <v>120</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+      <c r="I4">
+        <v>25.5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1">
-        <v>115</v>
-      </c>
-      <c r="G1">
-        <v>168</v>
-      </c>
-      <c r="H1">
+      <c r="F5">
+        <v>81</v>
+      </c>
+      <c r="G5">
+        <v>120</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+      <c r="I5">
+        <v>25.5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
         <v>54</v>
       </c>
-      <c r="I1">
+      <c r="F6">
+        <v>81</v>
+      </c>
+      <c r="G6">
+        <v>120</v>
+      </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <v>25.5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>54</v>
       </c>
-      <c r="J1" t="s">
-        <v>142</v>
-      </c>
-      <c r="K1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2">
-        <v>172</v>
-      </c>
-      <c r="C2">
-        <v>212</v>
-      </c>
-      <c r="D2">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2">
-        <v>103</v>
-      </c>
-      <c r="G2">
-        <v>143</v>
-      </c>
-      <c r="H2">
-        <v>41</v>
-      </c>
-      <c r="I2">
-        <v>41</v>
-      </c>
-      <c r="J2" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" t="s">
-        <v>146</v>
-      </c>
-      <c r="L2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3">
-        <v>150</v>
-      </c>
-      <c r="C3">
-        <v>187</v>
-      </c>
-      <c r="D3">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3">
-        <v>532</v>
-      </c>
-      <c r="G3">
-        <v>569</v>
-      </c>
-      <c r="H3">
-        <v>38</v>
-      </c>
-      <c r="I3">
-        <v>38</v>
-      </c>
-      <c r="J3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K3" t="s">
-        <v>144</v>
-      </c>
-      <c r="L3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>34</v>
-      </c>
-      <c r="D4">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>124</v>
-      </c>
-      <c r="G4">
-        <v>157</v>
-      </c>
-      <c r="H4">
-        <v>34</v>
-      </c>
-      <c r="I4">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>142</v>
-      </c>
-      <c r="K4" t="s">
-        <v>149</v>
-      </c>
-      <c r="L4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>133</v>
-      </c>
-      <c r="C5">
-        <v>165</v>
-      </c>
-      <c r="D5">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5">
+      <c r="F7">
+        <v>81</v>
+      </c>
+      <c r="G7">
+        <v>120</v>
+      </c>
+      <c r="H7">
         <v>40</v>
       </c>
-      <c r="G5">
-        <v>72</v>
-      </c>
-      <c r="H5">
-        <v>33</v>
-      </c>
-      <c r="I5">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>142</v>
-      </c>
-      <c r="K5" t="s">
-        <v>151</v>
-      </c>
-      <c r="L5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="I7">
+        <v>25.5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8">
+        <v>81</v>
+      </c>
+      <c r="G8">
+        <v>120</v>
+      </c>
+      <c r="H8">
         <v>40</v>
       </c>
-      <c r="B6">
-        <v>24</v>
-      </c>
-      <c r="C6">
-        <v>48</v>
-      </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6">
-        <v>119</v>
-      </c>
-      <c r="G6">
-        <v>152</v>
-      </c>
-      <c r="H6">
-        <v>34</v>
-      </c>
-      <c r="I6">
-        <v>29.5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K6" t="s">
-        <v>149</v>
-      </c>
-      <c r="L6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>29</v>
-      </c>
-      <c r="D7">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>65</v>
-      </c>
-      <c r="G7">
-        <v>93</v>
-      </c>
-      <c r="H7">
-        <v>29</v>
-      </c>
-      <c r="I7">
-        <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B8">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>42</v>
-      </c>
-      <c r="D8">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8">
-        <v>15</v>
-      </c>
-      <c r="G8">
-        <v>43</v>
-      </c>
-      <c r="H8">
-        <v>29</v>
-      </c>
       <c r="I8">
-        <v>29</v>
+        <v>25.5</v>
       </c>
       <c r="J8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>64</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>11</v>
@@ -1132,30 +1147,30 @@
         <v>54</v>
       </c>
       <c r="F9">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="G9">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="H9">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I9">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="J9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>11</v>
@@ -1164,158 +1179,158 @@
         <v>54</v>
       </c>
       <c r="F10">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="G10">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="H10">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I10">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="J10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B11">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="F11">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G11">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H11">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I11">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="J11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="F12">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12">
+        <v>117</v>
+      </c>
+      <c r="H12">
+        <v>38</v>
+      </c>
+      <c r="I12">
+        <v>24.5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>120</v>
       </c>
-      <c r="H12">
-        <v>40</v>
-      </c>
-      <c r="I12">
-        <v>25.5</v>
-      </c>
-      <c r="J12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>125</v>
-      </c>
       <c r="B13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="F13">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H13">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I13">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="J13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="F14">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H14">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I14">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="J14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B15">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C15">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1336,62 +1351,62 @@
         <v>24.5</v>
       </c>
       <c r="J15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="B16">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C16">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D16">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="F16">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="G16">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="H16">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I16">
-        <v>24.5</v>
+        <v>23</v>
       </c>
       <c r="J16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="F17">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="G17">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="H17">
         <v>38</v>
@@ -1400,933 +1415,1108 @@
         <v>24.5</v>
       </c>
       <c r="J17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>58</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C18">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D18">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="F18">
+        <v>48</v>
+      </c>
+      <c r="G18">
         <v>80</v>
       </c>
-      <c r="G18">
-        <v>117</v>
-      </c>
       <c r="H18">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I18">
-        <v>24.5</v>
+        <v>22</v>
       </c>
       <c r="J18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>82</v>
+      </c>
+      <c r="C19">
+        <v>103</v>
+      </c>
+      <c r="D19">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19">
+        <v>122</v>
+      </c>
+      <c r="G19">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B19">
-        <v>11</v>
-      </c>
-      <c r="C19">
+      <c r="H19">
         <v>21</v>
       </c>
-      <c r="D19">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19">
-        <v>80</v>
-      </c>
-      <c r="G19">
-        <v>117</v>
-      </c>
-      <c r="H19">
-        <v>38</v>
-      </c>
       <c r="I19">
-        <v>24.5</v>
+        <v>21.5</v>
       </c>
       <c r="J19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D20">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F20">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="G20">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="H20">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I20">
-        <v>24.5</v>
+        <v>17</v>
       </c>
       <c r="J20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C21">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D21">
         <v>11</v>
       </c>
       <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21">
+        <v>58</v>
+      </c>
+      <c r="G21">
+        <v>80</v>
+      </c>
+      <c r="H21">
+        <v>23</v>
+      </c>
+      <c r="I21">
+        <v>17</v>
+      </c>
+      <c r="J21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
         <v>54</v>
       </c>
-      <c r="F21">
-        <v>107</v>
-      </c>
-      <c r="G21">
-        <v>144</v>
-      </c>
-      <c r="H21">
-        <v>38</v>
-      </c>
-      <c r="I21">
-        <v>24.5</v>
-      </c>
-      <c r="J21" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22">
-        <v>18</v>
-      </c>
-      <c r="C22">
-        <v>28</v>
-      </c>
-      <c r="D22">
-        <v>11</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D23">
         <v>54</v>
       </c>
-      <c r="F22">
-        <v>107</v>
-      </c>
-      <c r="G22">
-        <v>144</v>
-      </c>
-      <c r="H22">
-        <v>38</v>
-      </c>
-      <c r="I22">
-        <v>24.5</v>
-      </c>
-      <c r="J22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23">
-        <v>33</v>
-      </c>
-      <c r="C23">
-        <v>42</v>
-      </c>
-      <c r="D23">
-        <v>10</v>
-      </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="F23">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="G23">
-        <v>117</v>
+        <v>168</v>
       </c>
       <c r="H23">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="I23">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="J23" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" t="s">
+        <v>143</v>
+      </c>
+      <c r="L23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>172</v>
       </c>
       <c r="C24">
-        <v>38</v>
+        <v>212</v>
       </c>
       <c r="D24">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="F24">
-        <v>1644</v>
+        <v>103</v>
       </c>
       <c r="G24">
-        <v>1671</v>
+        <v>143</v>
       </c>
       <c r="H24">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="I24">
-        <v>22.5</v>
+        <v>41</v>
       </c>
       <c r="J24" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" t="s">
+        <v>145</v>
+      </c>
+      <c r="L24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>136</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>150</v>
       </c>
       <c r="C25">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="D25">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
       <c r="F25">
-        <v>48</v>
+        <v>532</v>
       </c>
       <c r="G25">
-        <v>80</v>
+        <v>569</v>
       </c>
       <c r="H25">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I25">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="J25" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" t="s">
+        <v>143</v>
+      </c>
+      <c r="L25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>2</v>
       </c>
       <c r="B26">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>124</v>
+      </c>
+      <c r="G26">
+        <v>157</v>
+      </c>
+      <c r="H26">
+        <v>34</v>
+      </c>
+      <c r="I26">
+        <v>34</v>
+      </c>
+      <c r="J26" t="s">
+        <v>142</v>
+      </c>
+      <c r="K26" t="s">
+        <v>148</v>
+      </c>
+      <c r="L26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>133</v>
+      </c>
+      <c r="C27">
+        <v>165</v>
+      </c>
+      <c r="D27">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>40</v>
+      </c>
+      <c r="G27">
+        <v>72</v>
+      </c>
+      <c r="H27">
+        <v>33</v>
+      </c>
+      <c r="I27">
+        <v>33</v>
+      </c>
+      <c r="J27" t="s">
+        <v>142</v>
+      </c>
+      <c r="K27" t="s">
+        <v>150</v>
+      </c>
+      <c r="L27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>48</v>
+      </c>
+      <c r="D28">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28">
+        <v>119</v>
+      </c>
+      <c r="G28">
+        <v>152</v>
+      </c>
+      <c r="H28">
+        <v>34</v>
+      </c>
+      <c r="I28">
+        <v>29.5</v>
+      </c>
+      <c r="J28" t="s">
+        <v>142</v>
+      </c>
+      <c r="K28" t="s">
+        <v>148</v>
+      </c>
+      <c r="L28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>65</v>
+      </c>
+      <c r="G29">
+        <v>93</v>
+      </c>
+      <c r="H29">
+        <v>29</v>
+      </c>
+      <c r="I29">
+        <v>29</v>
+      </c>
+      <c r="J29" t="s">
+        <v>142</v>
+      </c>
+      <c r="K29" t="s">
+        <v>143</v>
+      </c>
+      <c r="L29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>42</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F30">
+        <v>15</v>
+      </c>
+      <c r="G30">
+        <v>43</v>
+      </c>
+      <c r="H30">
+        <v>29</v>
+      </c>
+      <c r="I30">
+        <v>29</v>
+      </c>
+      <c r="J30" t="s">
+        <v>142</v>
+      </c>
+      <c r="K30" t="s">
+        <v>143</v>
+      </c>
+      <c r="L30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31">
+        <v>81</v>
+      </c>
+      <c r="G31">
+        <v>120</v>
+      </c>
+      <c r="H31">
+        <v>40</v>
+      </c>
+      <c r="I31">
+        <v>25.5</v>
+      </c>
+      <c r="J31" t="s">
+        <v>142</v>
+      </c>
+      <c r="K31" t="s">
+        <v>157</v>
+      </c>
+      <c r="L31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32">
+        <v>1644</v>
+      </c>
+      <c r="G32">
+        <v>1671</v>
+      </c>
+      <c r="H32">
+        <v>28</v>
+      </c>
+      <c r="I32">
+        <v>22.5</v>
+      </c>
+      <c r="J32" t="s">
+        <v>142</v>
+      </c>
+      <c r="K32" t="s">
+        <v>143</v>
+      </c>
+      <c r="L32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>23</v>
+      </c>
+      <c r="D33">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33">
+        <v>48</v>
+      </c>
+      <c r="G33">
+        <v>80</v>
+      </c>
+      <c r="H33">
+        <v>33</v>
+      </c>
+      <c r="I33">
+        <v>22</v>
+      </c>
+      <c r="J33" t="s">
+        <v>142</v>
+      </c>
+      <c r="K33" t="s">
+        <v>157</v>
+      </c>
+      <c r="L33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>28</v>
+      </c>
+      <c r="C34">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34">
+        <v>191</v>
+      </c>
+      <c r="G34">
+        <v>217</v>
+      </c>
+      <c r="H34">
+        <v>27</v>
+      </c>
+      <c r="I34">
+        <v>21</v>
+      </c>
+      <c r="J34" t="s">
+        <v>142</v>
+      </c>
+      <c r="K34" t="s">
+        <v>150</v>
+      </c>
+      <c r="L34" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>35</v>
+      </c>
+      <c r="D35">
+        <v>21</v>
+      </c>
+      <c r="E35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35">
+        <v>289</v>
+      </c>
+      <c r="G35">
+        <v>309</v>
+      </c>
+      <c r="H35">
+        <v>21</v>
+      </c>
+      <c r="I35">
+        <v>21</v>
+      </c>
+      <c r="J35" t="s">
+        <v>142</v>
+      </c>
+      <c r="K35" t="s">
+        <v>143</v>
+      </c>
+      <c r="L35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>134</v>
       </c>
-      <c r="D26">
-        <v>58</v>
-      </c>
-      <c r="E26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26">
-        <v>85</v>
-      </c>
-      <c r="G26">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>135</v>
+      </c>
+      <c r="F36">
+        <v>33</v>
+      </c>
+      <c r="G36">
+        <v>52</v>
+      </c>
+      <c r="H36">
+        <v>20</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+      <c r="J36" t="s">
         <v>142</v>
       </c>
-      <c r="H26">
-        <v>58</v>
-      </c>
-      <c r="I26">
-        <v>58</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K36" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <v>11</v>
-      </c>
-      <c r="C27">
-        <v>60</v>
-      </c>
-      <c r="D27">
-        <v>50</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>82</v>
-      </c>
-      <c r="G27">
-        <v>131</v>
-      </c>
-      <c r="H27">
-        <v>50</v>
-      </c>
-      <c r="I27">
-        <v>50</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="L36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>28</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37">
+        <v>224</v>
+      </c>
+      <c r="G37">
+        <v>243</v>
+      </c>
+      <c r="H37">
+        <v>20</v>
+      </c>
+      <c r="I37">
+        <v>20</v>
+      </c>
+      <c r="J37" t="s">
+        <v>142</v>
+      </c>
+      <c r="K37" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28">
-        <v>9</v>
-      </c>
-      <c r="C28">
-        <v>38</v>
-      </c>
-      <c r="D28">
-        <v>30</v>
-      </c>
-      <c r="E28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28">
-        <v>28</v>
-      </c>
-      <c r="G28">
-        <v>57</v>
-      </c>
-      <c r="H28">
-        <v>30</v>
-      </c>
-      <c r="I28">
-        <v>30</v>
-      </c>
-      <c r="J28" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29">
-        <v>13</v>
-      </c>
-      <c r="C29">
-        <v>23</v>
-      </c>
-      <c r="D29">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29">
-        <v>48</v>
-      </c>
-      <c r="G29">
-        <v>80</v>
-      </c>
-      <c r="H29">
-        <v>33</v>
-      </c>
-      <c r="I29">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30">
-        <v>82</v>
-      </c>
-      <c r="C30">
-        <v>103</v>
-      </c>
-      <c r="D30">
-        <v>22</v>
-      </c>
-      <c r="E30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30">
-        <v>122</v>
-      </c>
-      <c r="G30">
-        <v>142</v>
-      </c>
-      <c r="H30">
-        <v>21</v>
-      </c>
-      <c r="I30">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
-        <v>28</v>
-      </c>
-      <c r="C31">
-        <v>42</v>
-      </c>
-      <c r="D31">
-        <v>15</v>
-      </c>
-      <c r="E31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31">
-        <v>191</v>
-      </c>
-      <c r="G31">
-        <v>217</v>
-      </c>
-      <c r="H31">
-        <v>27</v>
-      </c>
-      <c r="I31">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <v>15</v>
-      </c>
-      <c r="C32">
-        <v>35</v>
-      </c>
-      <c r="D32">
-        <v>21</v>
-      </c>
-      <c r="E32" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32">
-        <v>289</v>
-      </c>
-      <c r="G32">
-        <v>309</v>
-      </c>
-      <c r="H32">
-        <v>21</v>
-      </c>
-      <c r="I32">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>20</v>
-      </c>
-      <c r="D33">
-        <v>20</v>
-      </c>
-      <c r="E33" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33">
-        <v>33</v>
-      </c>
-      <c r="G33">
-        <v>52</v>
-      </c>
-      <c r="H33">
-        <v>20</v>
-      </c>
-      <c r="I33">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34">
-        <v>9</v>
-      </c>
-      <c r="C34">
-        <v>28</v>
-      </c>
-      <c r="D34">
-        <v>20</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34">
-        <v>224</v>
-      </c>
-      <c r="G34">
-        <v>243</v>
-      </c>
-      <c r="H34">
-        <v>20</v>
-      </c>
-      <c r="I34">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="L37" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>132</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>20</v>
-      </c>
-      <c r="D35">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
-        <v>133</v>
-      </c>
-      <c r="F35">
-        <v>4</v>
-      </c>
-      <c r="G35">
-        <v>23</v>
-      </c>
-      <c r="H35">
-        <v>20</v>
-      </c>
-      <c r="I35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36">
-        <v>25</v>
-      </c>
-      <c r="C36">
-        <v>40</v>
-      </c>
-      <c r="D36">
-        <v>16</v>
-      </c>
-      <c r="E36" t="s">
-        <v>23</v>
-      </c>
-      <c r="F36">
-        <v>290</v>
-      </c>
-      <c r="G36">
-        <v>311</v>
-      </c>
-      <c r="H36">
-        <v>22</v>
-      </c>
-      <c r="I36">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>128</v>
-      </c>
-      <c r="B37">
-        <v>11</v>
-      </c>
-      <c r="C37">
-        <v>29</v>
-      </c>
-      <c r="D37">
-        <v>19</v>
-      </c>
-      <c r="E37" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37">
-        <v>502</v>
-      </c>
-      <c r="G37">
-        <v>520</v>
-      </c>
-      <c r="H37">
-        <v>19</v>
-      </c>
-      <c r="I37">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>10</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D38">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="F38">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="G38">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="H38">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I38">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="J38" t="s">
+        <v>142</v>
+      </c>
+      <c r="K38" t="s">
+        <v>143</v>
+      </c>
+      <c r="L38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C39">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D39">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F39">
-        <v>11</v>
+        <v>290</v>
       </c>
       <c r="G39">
-        <v>29</v>
+        <v>311</v>
       </c>
       <c r="H39">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I39">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>142</v>
+      </c>
+      <c r="K39" t="s">
+        <v>148</v>
+      </c>
+      <c r="L39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="B40">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D40">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="F40">
-        <v>93</v>
+        <v>502</v>
       </c>
       <c r="G40">
-        <v>120</v>
+        <v>520</v>
       </c>
       <c r="H40">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I40">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J40" t="s">
+        <v>142</v>
+      </c>
+      <c r="K40" t="s">
+        <v>143</v>
+      </c>
+      <c r="L40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D41">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E41" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="F41">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="G41">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="H41">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I41">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J41" t="s">
+        <v>142</v>
+      </c>
+      <c r="K41" t="s">
+        <v>143</v>
+      </c>
+      <c r="L41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D42">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E42" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="F42">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="G42">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="H42">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I42">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="J42" t="s">
+        <v>142</v>
+      </c>
+      <c r="K42" t="s">
+        <v>143</v>
+      </c>
+      <c r="L42" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C43">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D43">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="F43">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="G43">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="H43">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I43">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="J43" t="s">
+        <v>142</v>
+      </c>
+      <c r="K43" t="s">
+        <v>157</v>
+      </c>
+      <c r="L43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D44">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E44" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44">
+        <v>15</v>
+      </c>
+      <c r="G44">
+        <v>32</v>
+      </c>
+      <c r="H44">
+        <v>18</v>
+      </c>
+      <c r="I44">
+        <v>18</v>
+      </c>
+      <c r="J44" t="s">
+        <v>142</v>
+      </c>
+      <c r="K44" t="s">
+        <v>148</v>
+      </c>
+      <c r="L44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>17</v>
+      </c>
+      <c r="D45">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
+        <v>85</v>
+      </c>
+      <c r="F45">
+        <v>69</v>
+      </c>
+      <c r="G45">
+        <v>85</v>
+      </c>
+      <c r="H45">
+        <v>17</v>
+      </c>
+      <c r="I45">
+        <v>17</v>
+      </c>
+      <c r="J45" t="s">
+        <v>142</v>
+      </c>
+      <c r="K45" t="s">
+        <v>148</v>
+      </c>
+      <c r="L45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>17</v>
+      </c>
+      <c r="D46">
+        <v>17</v>
+      </c>
+      <c r="E46" t="s">
         <v>102</v>
       </c>
-      <c r="F44">
+      <c r="F46">
         <v>45</v>
       </c>
-      <c r="G44">
+      <c r="G46">
         <v>61</v>
       </c>
-      <c r="H44">
-        <v>17</v>
-      </c>
-      <c r="I44">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="H46">
+        <v>17</v>
+      </c>
+      <c r="I46">
+        <v>17</v>
+      </c>
+      <c r="J46" t="s">
+        <v>142</v>
+      </c>
+      <c r="K46" t="s">
+        <v>148</v>
+      </c>
+      <c r="L46" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>52</v>
       </c>
-      <c r="B45">
+      <c r="B47">
         <v>7</v>
       </c>
-      <c r="C45">
-        <v>17</v>
-      </c>
-      <c r="D45">
+      <c r="C47">
+        <v>17</v>
+      </c>
+      <c r="D47">
         <v>11</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E47" t="s">
         <v>49</v>
       </c>
-      <c r="F45">
+      <c r="F47">
         <v>58</v>
       </c>
-      <c r="G45">
+      <c r="G47">
         <v>80</v>
       </c>
-      <c r="H45">
+      <c r="H47">
         <v>23</v>
       </c>
-      <c r="I45">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46">
-        <v>34</v>
-      </c>
-      <c r="C46">
-        <v>44</v>
-      </c>
-      <c r="D46">
-        <v>11</v>
-      </c>
-      <c r="E46" t="s">
-        <v>49</v>
-      </c>
-      <c r="F46">
-        <v>58</v>
-      </c>
-      <c r="G46">
+      <c r="I47">
+        <v>17</v>
+      </c>
+      <c r="J47" t="s">
+        <v>142</v>
+      </c>
+      <c r="K47" t="s">
+        <v>157</v>
+      </c>
+      <c r="L47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48">
+        <v>64</v>
+      </c>
+      <c r="C48">
         <v>80</v>
       </c>
-      <c r="H46">
-        <v>23</v>
-      </c>
-      <c r="I46">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47">
-        <v>64</v>
-      </c>
-      <c r="C47">
-        <v>80</v>
-      </c>
-      <c r="D47">
-        <v>17</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="D48">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
         <v>96</v>
       </c>
-      <c r="F47">
+      <c r="F48">
         <v>21</v>
       </c>
-      <c r="G47">
+      <c r="G48">
         <v>37</v>
-      </c>
-      <c r="H47">
-        <v>17</v>
-      </c>
-      <c r="I47">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>38</v>
-      </c>
-      <c r="B48">
-        <v>23</v>
-      </c>
-      <c r="C48">
-        <v>39</v>
-      </c>
-      <c r="D48">
-        <v>17</v>
-      </c>
-      <c r="E48" t="s">
-        <v>39</v>
-      </c>
-      <c r="F48">
-        <v>27</v>
-      </c>
-      <c r="G48">
-        <v>43</v>
       </c>
       <c r="H48">
         <v>17</v>
@@ -2337,25 +2527,25 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C49">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D49">
         <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="F49">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G49">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H49">
         <v>17</v>
@@ -2366,28 +2556,28 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="B50">
+        <v>13</v>
+      </c>
+      <c r="C50">
+        <v>29</v>
+      </c>
+      <c r="D50">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50">
+        <v>31</v>
+      </c>
+      <c r="G50">
         <v>47</v>
       </c>
-      <c r="C50">
-        <v>59</v>
-      </c>
-      <c r="D50">
-        <v>13</v>
-      </c>
-      <c r="E50" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50">
-        <v>32</v>
-      </c>
-      <c r="G50">
-        <v>52</v>
-      </c>
       <c r="H50">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I50">
         <v>17</v>
@@ -2395,28 +2585,28 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="C51">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D51">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E51" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="F51">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G51">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="H51">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I51">
         <v>17</v>
@@ -2424,25 +2614,25 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C52">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D52">
         <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="F52">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G52">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H52">
         <v>17</v>
@@ -2453,28 +2643,28 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="B53">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C53">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D53">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="F53">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="G53">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="H53">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I53">
         <v>17</v>
@@ -2482,13 +2672,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C54">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D54">
         <v>11</v>
@@ -2511,28 +2701,28 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C55">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D55">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="F55">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="G55">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="H55">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I55">
         <v>17</v>
@@ -2540,28 +2730,28 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D56">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="F56">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G56">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H56">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I56">
         <v>17</v>
@@ -2569,28 +2759,28 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="B57">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C57">
+        <v>20</v>
+      </c>
+      <c r="D57">
+        <v>16</v>
+      </c>
+      <c r="E57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57">
+        <v>45</v>
+      </c>
+      <c r="G57">
+        <v>62</v>
+      </c>
+      <c r="H57">
         <v>18</v>
-      </c>
-      <c r="D57">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
-        <v>49</v>
-      </c>
-      <c r="F57">
-        <v>58</v>
-      </c>
-      <c r="G57">
-        <v>80</v>
-      </c>
-      <c r="H57">
-        <v>23</v>
       </c>
       <c r="I57">
         <v>17</v>
@@ -2598,28 +2788,28 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C58">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D58">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F58">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G58">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H58">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I58">
         <v>17</v>
@@ -2627,7 +2817,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2639,13 +2829,13 @@
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="F59">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G59">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="H59">
         <v>17</v>
@@ -2656,7 +2846,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2668,13 +2858,13 @@
         <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F60">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="G60">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="H60">
         <v>17</v>
@@ -2685,28 +2875,28 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C61">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D61">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="F61">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="G61">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H61">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I61">
         <v>17</v>
@@ -2714,28 +2904,28 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="B62">
+        <v>4</v>
+      </c>
+      <c r="C62">
         <v>14</v>
       </c>
-      <c r="C62">
-        <v>30</v>
-      </c>
       <c r="D62">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E62" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="F62">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G62">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="H62">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I62">
         <v>17</v>
@@ -2743,28 +2933,28 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C63">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D63">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E63" t="s">
+        <v>102</v>
+      </c>
+      <c r="F63">
         <v>45</v>
       </c>
-      <c r="F63">
-        <v>32</v>
-      </c>
       <c r="G63">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="H63">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I63">
         <v>17</v>
@@ -2772,13 +2962,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
         <v>14</v>
-      </c>
-      <c r="C64">
-        <v>26</v>
       </c>
       <c r="D64">
         <v>13</v>
@@ -2801,28 +2991,28 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B65">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C65">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D65">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E65" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="F65">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="G65">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="H65">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I65">
         <v>17</v>
@@ -2830,28 +3020,28 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C66">
         <v>17</v>
       </c>
       <c r="D66">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F66">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="G66">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="H66">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I66">
         <v>17</v>
@@ -2859,7 +3049,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2871,13 +3061,13 @@
         <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>17</v>
+        <v>102</v>
       </c>
       <c r="F67">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G67">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="H67">
         <v>17</v>
@@ -2888,25 +3078,25 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="B68">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="D68">
         <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>131</v>
+        <v>17</v>
       </c>
       <c r="F68">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G68">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H68">
         <v>17</v>
@@ -2917,28 +3107,28 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>130</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C69">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="D69">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="F69">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="G69">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="H69">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I69">
         <v>17</v>
@@ -2946,42 +3136,42 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B70">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E70" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="F70">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="G70">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="H70">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I70">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B71">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C71">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D71">
         <v>10</v>
@@ -3004,13 +3194,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C72">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D72">
         <v>10</v>
@@ -3033,28 +3223,28 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B73">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C73">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="D73">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F73">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="G73">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="H73">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I73">
         <v>16</v>
@@ -3062,28 +3252,28 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="B74">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C74">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="D74">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E74" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F74">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G74">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="H74">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I74">
         <v>16</v>
@@ -3091,13 +3281,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B75">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C75">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D75">
         <v>10</v>
@@ -3120,13 +3310,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B76">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D76">
         <v>10</v>
@@ -3149,28 +3339,28 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C77">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D77">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E77" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F77">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="G77">
+        <v>79</v>
+      </c>
+      <c r="H77">
         <v>22</v>
-      </c>
-      <c r="H77">
-        <v>16</v>
       </c>
       <c r="I77">
         <v>16</v>
@@ -3178,25 +3368,25 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>16</v>
+      </c>
+      <c r="D78">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
         <v>27</v>
       </c>
-      <c r="C78">
-        <v>42</v>
-      </c>
-      <c r="D78">
-        <v>16</v>
-      </c>
-      <c r="E78" t="s">
-        <v>101</v>
-      </c>
       <c r="F78">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G78">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="H78">
         <v>16</v>
@@ -3207,28 +3397,28 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C79">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D79">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="F79">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="G79">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="H79">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I79">
         <v>16</v>
@@ -3236,13 +3426,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B80">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C80">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D80">
         <v>10</v>
@@ -3265,7 +3455,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B81">
         <v>10</v>
@@ -3294,13 +3484,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C82">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D82">
         <v>10</v>
@@ -3323,28 +3513,28 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C83">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D83">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E83" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F83">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="G83">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="H83">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I83">
         <v>16</v>
@@ -3352,7 +3542,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -3364,13 +3554,13 @@
         <v>16</v>
       </c>
       <c r="E84" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F84">
-        <v>399</v>
+        <v>1</v>
       </c>
       <c r="G84">
-        <v>414</v>
+        <v>16</v>
       </c>
       <c r="H84">
         <v>16</v>
@@ -3381,28 +3571,28 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="B85">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C85">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D85">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E85" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F85">
-        <v>58</v>
+        <v>399</v>
       </c>
       <c r="G85">
-        <v>79</v>
+        <v>414</v>
       </c>
       <c r="H85">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I85">
         <v>16</v>
@@ -3410,13 +3600,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B86">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C86">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D86">
         <v>10</v>
@@ -3439,28 +3629,28 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C87">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D87">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="F87">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G87">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H87">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I87">
         <v>16</v>
@@ -3468,28 +3658,28 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>28</v>
+        <v>126</v>
       </c>
       <c r="B88">
         <v>1</v>
       </c>
       <c r="C88">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D88">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E88" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="F88">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="G88">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="H88">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I88">
         <v>16</v>
@@ -3497,57 +3687,57 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="B89">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="D89">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E89" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="F89">
-        <v>324</v>
+        <v>1</v>
       </c>
       <c r="G89">
-        <v>345</v>
+        <v>16</v>
       </c>
       <c r="H89">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I89">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B90">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="C90">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="D90">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="F90">
-        <v>37</v>
+        <v>324</v>
       </c>
       <c r="G90">
-        <v>55</v>
+        <v>345</v>
       </c>
       <c r="H90">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I90">
         <v>15</v>
@@ -3555,28 +3745,28 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="B91">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D91">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E91" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="F91">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="G91">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="H91">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I91">
         <v>15</v>
@@ -3584,28 +3774,28 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="B92">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C92">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D92">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E92" t="s">
+        <v>105</v>
+      </c>
+      <c r="F92">
+        <v>67</v>
+      </c>
+      <c r="G92">
         <v>83</v>
       </c>
-      <c r="F92">
-        <v>197</v>
-      </c>
-      <c r="G92">
-        <v>215</v>
-      </c>
       <c r="H92">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I92">
         <v>15</v>
@@ -3613,25 +3803,25 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B93">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="C93">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="D93">
         <v>11</v>
       </c>
       <c r="E93" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F93">
-        <v>93</v>
+        <v>197</v>
       </c>
       <c r="G93">
-        <v>111</v>
+        <v>215</v>
       </c>
       <c r="H93">
         <v>19</v>
@@ -3642,13 +3832,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="B94">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="C94">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="D94">
         <v>11</v>
@@ -3666,6 +3856,35 @@
         <v>19</v>
       </c>
       <c r="I94">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95">
+        <v>16</v>
+      </c>
+      <c r="C95">
+        <v>26</v>
+      </c>
+      <c r="D95">
+        <v>11</v>
+      </c>
+      <c r="E95" t="s">
+        <v>92</v>
+      </c>
+      <c r="F95">
+        <v>93</v>
+      </c>
+      <c r="G95">
+        <v>111</v>
+      </c>
+      <c r="H95">
+        <v>19</v>
+      </c>
+      <c r="I95">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the results to have 50 files for manual investigation
</commit_message>
<xml_diff>
--- a/manual/simian_default_combined.xlsx
+++ b/manual/simian_default_combined.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="6380" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="simian_default_combined" sheetId="1" r:id="rId1"/>
@@ -854,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -874,7 +874,7 @@
     <col min="12" max="12" width="69.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>127</v>
       </c>
@@ -906,431 +906,479 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>54</v>
+      </c>
+      <c r="D2">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>115</v>
+      </c>
+      <c r="G2">
+        <v>168</v>
+      </c>
+      <c r="H2">
+        <v>54</v>
+      </c>
+      <c r="I2">
+        <v>54</v>
+      </c>
+      <c r="J2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>60</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>50</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>82</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>131</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>50</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>50</v>
-      </c>
-      <c r="J2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>38</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3">
-        <v>28</v>
-      </c>
-      <c r="G3">
-        <v>57</v>
-      </c>
-      <c r="H3">
-        <v>30</v>
-      </c>
-      <c r="I3">
-        <v>30</v>
       </c>
       <c r="J3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4">
+        <v>172</v>
+      </c>
+      <c r="C4">
+        <v>212</v>
+      </c>
+      <c r="D4">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4">
+        <v>103</v>
+      </c>
+      <c r="G4">
+        <v>143</v>
+      </c>
+      <c r="H4">
+        <v>41</v>
+      </c>
+      <c r="I4">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5">
+        <v>150</v>
+      </c>
+      <c r="C5">
+        <v>187</v>
+      </c>
+      <c r="D5">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5">
+        <v>532</v>
+      </c>
+      <c r="G5">
+        <v>569</v>
+      </c>
+      <c r="H5">
+        <v>38</v>
+      </c>
+      <c r="I5">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>142</v>
+      </c>
+      <c r="K5" t="s">
+        <v>143</v>
+      </c>
+      <c r="L5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>124</v>
+      </c>
+      <c r="G6">
+        <v>157</v>
+      </c>
+      <c r="H6">
+        <v>34</v>
+      </c>
+      <c r="I6">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>133</v>
+      </c>
+      <c r="C7">
+        <v>165</v>
+      </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <v>72</v>
+      </c>
+      <c r="H7">
+        <v>33</v>
+      </c>
+      <c r="I7">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>142</v>
+      </c>
+      <c r="K7" t="s">
+        <v>150</v>
+      </c>
+      <c r="L7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>28</v>
+      </c>
+      <c r="G8">
+        <v>57</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>48</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <v>119</v>
+      </c>
+      <c r="G9">
+        <v>152</v>
+      </c>
+      <c r="H9">
+        <v>34</v>
+      </c>
+      <c r="I9">
+        <v>29.5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K9" t="s">
+        <v>148</v>
+      </c>
+      <c r="L9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>65</v>
+      </c>
+      <c r="G10">
+        <v>93</v>
+      </c>
+      <c r="H10">
+        <v>29</v>
+      </c>
+      <c r="I10">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>142</v>
+      </c>
+      <c r="K10" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>43</v>
+      </c>
+      <c r="H11">
+        <v>29</v>
+      </c>
+      <c r="I11">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" t="s">
+        <v>143</v>
+      </c>
+      <c r="L11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>122</v>
       </c>
-      <c r="B4">
+      <c r="B12">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4">
-        <v>81</v>
-      </c>
-      <c r="G4">
-        <v>120</v>
-      </c>
-      <c r="H4">
-        <v>40</v>
-      </c>
-      <c r="I4">
-        <v>25.5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5">
-        <v>81</v>
-      </c>
-      <c r="G5">
-        <v>120</v>
-      </c>
-      <c r="H5">
-        <v>40</v>
-      </c>
-      <c r="I5">
-        <v>25.5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6">
-        <v>81</v>
-      </c>
-      <c r="G6">
-        <v>120</v>
-      </c>
-      <c r="H6">
-        <v>40</v>
-      </c>
-      <c r="I6">
-        <v>25.5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7">
-        <v>81</v>
-      </c>
-      <c r="G7">
-        <v>120</v>
-      </c>
-      <c r="H7">
-        <v>40</v>
-      </c>
-      <c r="I7">
-        <v>25.5</v>
-      </c>
-      <c r="J7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8">
-        <v>81</v>
-      </c>
-      <c r="G8">
-        <v>120</v>
-      </c>
-      <c r="H8">
-        <v>40</v>
-      </c>
-      <c r="I8">
-        <v>25.5</v>
-      </c>
-      <c r="J8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>21</v>
-      </c>
-      <c r="D9">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9">
-        <v>107</v>
-      </c>
-      <c r="G9">
-        <v>144</v>
-      </c>
-      <c r="H9">
-        <v>38</v>
-      </c>
-      <c r="I9">
-        <v>24.5</v>
-      </c>
-      <c r="J9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>28</v>
-      </c>
-      <c r="D10">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10">
-        <v>107</v>
-      </c>
-      <c r="G10">
-        <v>144</v>
-      </c>
-      <c r="H10">
-        <v>38</v>
-      </c>
-      <c r="I10">
-        <v>24.5</v>
-      </c>
-      <c r="J10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>16</v>
-      </c>
-      <c r="D11">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11">
-        <v>80</v>
-      </c>
-      <c r="G11">
-        <v>117</v>
-      </c>
-      <c r="H11">
-        <v>38</v>
-      </c>
-      <c r="I11">
-        <v>24.5</v>
-      </c>
-      <c r="J11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
       <c r="C12">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="F12">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G12">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H12">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I12">
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="J12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C13">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="F13">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G13">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H13">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I13">
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="J13" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C14">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D14">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="F14">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G14">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H14">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I14">
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="J14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="B15">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>11</v>
@@ -1339,48 +1387,48 @@
         <v>54</v>
       </c>
       <c r="F15">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="G15">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="H15">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I15">
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="J15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="F16">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G16">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H16">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="I16">
-        <v>23</v>
+        <v>25.5</v>
       </c>
       <c r="J16" t="s">
         <v>156</v>
@@ -1388,13 +1436,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D17">
         <v>11</v>
@@ -1403,48 +1451,54 @@
         <v>54</v>
       </c>
       <c r="F17">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="G17">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="H17">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I17">
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="J17" t="s">
-        <v>156</v>
+        <v>142</v>
+      </c>
+      <c r="K17" t="s">
+        <v>157</v>
+      </c>
+      <c r="L17" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B18">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F18">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="G18">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="H18">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I18">
-        <v>22</v>
+        <v>24.5</v>
       </c>
       <c r="J18" t="s">
         <v>156</v>
@@ -1452,31 +1506,31 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B19">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="C19">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="D19">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F19">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="G19">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H19">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="I19">
-        <v>21.5</v>
+        <v>24.5</v>
       </c>
       <c r="J19" t="s">
         <v>156</v>
@@ -1484,31 +1538,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="F20">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="G20">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="H20">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="I20">
-        <v>17</v>
+        <v>24.5</v>
       </c>
       <c r="J20" t="s">
         <v>156</v>
@@ -1516,405 +1570,401 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="B21">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C21">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D21">
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="F21">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="G21">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="H21">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="I21">
-        <v>17</v>
+        <v>24.5</v>
       </c>
       <c r="J21" t="s">
         <v>156</v>
       </c>
     </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22">
+        <v>80</v>
+      </c>
+      <c r="G22">
+        <v>117</v>
+      </c>
+      <c r="H22">
+        <v>38</v>
+      </c>
+      <c r="I22">
+        <v>24.5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C23">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="D23">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="F23">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="G23">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="H23">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="I23">
-        <v>54</v>
+        <v>24.5</v>
       </c>
       <c r="J23" t="s">
-        <v>142</v>
-      </c>
-      <c r="K23" t="s">
-        <v>143</v>
-      </c>
-      <c r="L23" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="B24">
-        <v>172</v>
+        <v>18</v>
       </c>
       <c r="C24">
-        <v>212</v>
+        <v>28</v>
       </c>
       <c r="D24">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="F24">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G24">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H24">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I24">
-        <v>41</v>
+        <v>24.5</v>
       </c>
       <c r="J24" t="s">
-        <v>142</v>
-      </c>
-      <c r="K24" t="s">
-        <v>145</v>
-      </c>
-      <c r="L24" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>67</v>
       </c>
       <c r="B25">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="C25">
-        <v>187</v>
+        <v>15</v>
       </c>
       <c r="D25">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>137</v>
+        <v>54</v>
       </c>
       <c r="F25">
-        <v>532</v>
+        <v>107</v>
       </c>
       <c r="G25">
-        <v>569</v>
+        <v>144</v>
       </c>
       <c r="H25">
         <v>38</v>
       </c>
       <c r="I25">
-        <v>38</v>
+        <v>24.5</v>
       </c>
       <c r="J25" t="s">
-        <v>142</v>
-      </c>
-      <c r="K25" t="s">
-        <v>143</v>
-      </c>
-      <c r="L25" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C26">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D26">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F26">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="G26">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="H26">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I26">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>142</v>
-      </c>
-      <c r="K26" t="s">
-        <v>148</v>
-      </c>
-      <c r="L26" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="B27">
-        <v>133</v>
+        <v>22</v>
       </c>
       <c r="C27">
-        <v>165</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="F27">
-        <v>40</v>
+        <v>1644</v>
       </c>
       <c r="G27">
-        <v>72</v>
+        <v>1671</v>
       </c>
       <c r="H27">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I27">
-        <v>33</v>
+        <v>22.5</v>
       </c>
       <c r="J27" t="s">
         <v>142</v>
       </c>
       <c r="K27" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L27" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B28">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C28">
+        <v>23</v>
+      </c>
+      <c r="D28">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28">
         <v>48</v>
       </c>
-      <c r="D28">
-        <v>25</v>
-      </c>
-      <c r="E28" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28">
-        <v>119</v>
-      </c>
       <c r="G28">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="H28">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I28">
-        <v>29.5</v>
+        <v>22</v>
       </c>
       <c r="J28" t="s">
-        <v>142</v>
-      </c>
-      <c r="K28" t="s">
-        <v>148</v>
-      </c>
-      <c r="L28" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D29">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F29">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="G29">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="H29">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I29">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J29" t="s">
         <v>142</v>
       </c>
       <c r="K29" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="L29" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>36</v>
       </c>
       <c r="B30">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C30">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="D30">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E30" t="s">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="F30">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="G30">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="H30">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I30">
-        <v>29</v>
+        <v>21.5</v>
       </c>
       <c r="J30" t="s">
-        <v>142</v>
-      </c>
-      <c r="K30" t="s">
-        <v>143</v>
-      </c>
-      <c r="L30" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C31">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D31">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="F31">
-        <v>81</v>
+        <v>191</v>
       </c>
       <c r="G31">
-        <v>120</v>
+        <v>217</v>
       </c>
       <c r="H31">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I31">
-        <v>25.5</v>
+        <v>21</v>
       </c>
       <c r="J31" t="s">
         <v>142</v>
       </c>
       <c r="K31" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="L31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>34</v>
       </c>
       <c r="B32">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C32">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D32">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E32" t="s">
-        <v>141</v>
+        <v>35</v>
       </c>
       <c r="F32">
-        <v>1644</v>
+        <v>289</v>
       </c>
       <c r="G32">
-        <v>1671</v>
+        <v>309</v>
       </c>
       <c r="H32">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I32">
-        <v>22.5</v>
+        <v>21</v>
       </c>
       <c r="J32" t="s">
         <v>142</v>
@@ -1923,112 +1973,112 @@
         <v>143</v>
       </c>
       <c r="L32" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="B33">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D33">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>51</v>
+        <v>135</v>
       </c>
       <c r="F33">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="G33">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="H33">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="I33">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J33" t="s">
         <v>142</v>
       </c>
       <c r="K33" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="L33" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
         <v>28</v>
       </c>
-      <c r="C34">
-        <v>42</v>
-      </c>
       <c r="D34">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F34">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="G34">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="H34">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I34">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J34" t="s">
         <v>142</v>
       </c>
       <c r="K34" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L34" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="B35">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D35">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="F35">
-        <v>289</v>
+        <v>4</v>
       </c>
       <c r="G35">
-        <v>309</v>
+        <v>23</v>
       </c>
       <c r="H35">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I35">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J35" t="s">
         <v>142</v>
@@ -2037,74 +2087,74 @@
         <v>143</v>
       </c>
       <c r="L35" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C36">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D36">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
-        <v>135</v>
+        <v>23</v>
       </c>
       <c r="F36">
-        <v>33</v>
+        <v>290</v>
       </c>
       <c r="G36">
-        <v>52</v>
+        <v>311</v>
       </c>
       <c r="H36">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I36">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J36" t="s">
         <v>142</v>
       </c>
       <c r="K36" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="L36" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="B37">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C37">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>129</v>
       </c>
       <c r="F37">
-        <v>224</v>
+        <v>502</v>
       </c>
       <c r="G37">
-        <v>243</v>
+        <v>520</v>
       </c>
       <c r="H37">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I37">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J37" t="s">
         <v>142</v>
@@ -2113,36 +2163,36 @@
         <v>143</v>
       </c>
       <c r="L37" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>132</v>
+        <v>10</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D38">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="F38">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="G38">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="H38">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J38" t="s">
         <v>142</v>
@@ -2151,33 +2201,33 @@
         <v>143</v>
       </c>
       <c r="L38" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B39">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D39">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F39">
-        <v>290</v>
+        <v>11</v>
       </c>
       <c r="G39">
-        <v>311</v>
+        <v>29</v>
       </c>
       <c r="H39">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I39">
         <v>19</v>
@@ -2186,191 +2236,179 @@
         <v>142</v>
       </c>
       <c r="K39" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="L39" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="B40">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C40">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D40">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="F40">
-        <v>502</v>
+        <v>93</v>
       </c>
       <c r="G40">
-        <v>520</v>
+        <v>120</v>
       </c>
       <c r="H40">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="I40">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J40" t="s">
         <v>142</v>
       </c>
       <c r="K40" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="L40" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>118</v>
       </c>
       <c r="F41">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="G41">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="H41">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I41">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J41" t="s">
         <v>142</v>
       </c>
       <c r="K41" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="L41" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D42">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="F42">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="G42">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="H42">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I42">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J42" t="s">
-        <v>142</v>
-      </c>
-      <c r="K42" t="s">
-        <v>143</v>
-      </c>
-      <c r="L42" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
       <c r="B43">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C43">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D43">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F43">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="G43">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="H43">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I43">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J43" t="s">
-        <v>142</v>
-      </c>
-      <c r="K43" t="s">
-        <v>157</v>
-      </c>
-      <c r="L43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="F44">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="G44">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="H44">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I44">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J44" t="s">
         <v>142</v>
@@ -2379,12 +2417,12 @@
         <v>148</v>
       </c>
       <c r="L44" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2396,13 +2434,13 @@
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="F45">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="G45">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="H45">
         <v>17</v>
@@ -2417,33 +2455,33 @@
         <v>148</v>
       </c>
       <c r="L45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C46">
         <v>17</v>
       </c>
       <c r="D46">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="F46">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G46">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="H46">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I46">
         <v>17</v>
@@ -2452,71 +2490,62 @@
         <v>142</v>
       </c>
       <c r="K46" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="L46" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C47">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="D47">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="F47">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="G47">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="H47">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I47">
         <v>17</v>
-      </c>
-      <c r="J47" t="s">
-        <v>142</v>
-      </c>
-      <c r="K47" t="s">
-        <v>157</v>
-      </c>
-      <c r="L47" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="B48">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="C48">
-        <v>80</v>
+        <v>39</v>
       </c>
       <c r="D48">
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="F48">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G48">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H48">
         <v>17</v>
@@ -2527,25 +2556,25 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="B49">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C49">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D49">
         <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="F49">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G49">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H49">
         <v>17</v>
@@ -2556,28 +2585,28 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B50">
+        <v>47</v>
+      </c>
+      <c r="C50">
+        <v>59</v>
+      </c>
+      <c r="D50">
         <v>13</v>
       </c>
-      <c r="C50">
-        <v>29</v>
-      </c>
-      <c r="D50">
-        <v>17</v>
-      </c>
       <c r="E50" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="F50">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G50">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H50">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I50">
         <v>17</v>
@@ -2585,28 +2614,28 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B51">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C51">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="D51">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E51" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="F51">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G51">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="H51">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I51">
         <v>17</v>
@@ -2614,25 +2643,25 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B52">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C52">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D52">
         <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="F52">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G52">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H52">
         <v>17</v>
@@ -2643,28 +2672,28 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="B53">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C53">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D53">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
+        <v>49</v>
       </c>
       <c r="F53">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="G53">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="H53">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I53">
         <v>17</v>
@@ -2672,13 +2701,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B54">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C54">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D54">
         <v>11</v>
@@ -2701,28 +2730,28 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C55">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D55">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="F55">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="G55">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="H55">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I55">
         <v>17</v>
@@ -2730,28 +2759,28 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C56">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D56">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E56" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
       <c r="F56">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G56">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H56">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I56">
         <v>17</v>
@@ -2759,28 +2788,28 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57">
         <v>18</v>
       </c>
-      <c r="B57">
-        <v>5</v>
-      </c>
-      <c r="C57">
-        <v>20</v>
-      </c>
       <c r="D57">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E57" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="F57">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="G57">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H57">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I57">
         <v>17</v>
@@ -2788,28 +2817,28 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B58">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D58">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="F58">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="G58">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H58">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I58">
         <v>17</v>
@@ -2817,7 +2846,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2829,13 +2858,13 @@
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="F59">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="G59">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="H59">
         <v>17</v>
@@ -2846,7 +2875,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2858,13 +2887,13 @@
         <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="F60">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G60">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="H60">
         <v>17</v>
@@ -2875,28 +2904,28 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C61">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D61">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F61">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G61">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H61">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I61">
         <v>17</v>
@@ -2904,28 +2933,28 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="B62">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C62">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D62">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="F62">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="G62">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="H62">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I62">
         <v>17</v>
@@ -2933,28 +2962,28 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
         <v>14</v>
       </c>
-      <c r="C63">
-        <v>30</v>
-      </c>
       <c r="D63">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E63" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="F63">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G63">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="H63">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I63">
         <v>17</v>
@@ -2962,13 +2991,13 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C64">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D64">
         <v>13</v>
@@ -2991,28 +3020,28 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B65">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C65">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D65">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E65" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="F65">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="G65">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="H65">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I65">
         <v>17</v>
@@ -3020,28 +3049,28 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="B66">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>17</v>
       </c>
       <c r="D66">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="F66">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G66">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="H66">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I66">
         <v>17</v>
@@ -3049,7 +3078,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -3061,13 +3090,13 @@
         <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="F67">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G67">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H67">
         <v>17</v>
@@ -3078,25 +3107,25 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C68">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="D68">
         <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="F68">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G68">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H68">
         <v>17</v>
@@ -3107,28 +3136,28 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>59</v>
       </c>
       <c r="B69">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D69">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E69" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="F69">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="G69">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="H69">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I69">
         <v>17</v>
@@ -3136,42 +3165,42 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C70">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D70">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E70" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="F70">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="G70">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="H70">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I70">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B71">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C71">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D71">
         <v>10</v>
@@ -3194,13 +3223,13 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B72">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C72">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D72">
         <v>10</v>
@@ -3223,28 +3252,28 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="B73">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C73">
+        <v>60</v>
+      </c>
+      <c r="D73">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
         <v>21</v>
       </c>
-      <c r="D73">
-        <v>10</v>
-      </c>
-      <c r="E73" t="s">
-        <v>43</v>
-      </c>
       <c r="F73">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G73">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="H73">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I73">
         <v>16</v>
@@ -3252,28 +3281,28 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B74">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C74">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="D74">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E74" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F74">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="G74">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="H74">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I74">
         <v>16</v>
@@ -3281,13 +3310,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B75">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C75">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D75">
         <v>10</v>
@@ -3310,13 +3339,13 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B76">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C76">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D76">
         <v>10</v>
@@ -3339,28 +3368,28 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="B77">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C77">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D77">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E77" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F77">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="G77">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="H77">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I77">
         <v>16</v>
@@ -3368,25 +3397,25 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C78">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D78">
         <v>16</v>
       </c>
       <c r="E78" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="F78">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G78">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H78">
         <v>16</v>
@@ -3397,28 +3426,28 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B79">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C79">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D79">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E79" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="F79">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="G79">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="H79">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I79">
         <v>16</v>
@@ -3426,13 +3455,13 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B80">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C80">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D80">
         <v>10</v>
@@ -3455,7 +3484,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B81">
         <v>10</v>
@@ -3484,13 +3513,13 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B82">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C82">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D82">
         <v>10</v>
@@ -3513,28 +3542,28 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B83">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C83">
+        <v>16</v>
+      </c>
+      <c r="D83">
+        <v>16</v>
+      </c>
+      <c r="E83" t="s">
         <v>29</v>
       </c>
-      <c r="D83">
-        <v>10</v>
-      </c>
-      <c r="E83" t="s">
-        <v>43</v>
-      </c>
       <c r="F83">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="G83">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="H83">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I83">
         <v>16</v>
@@ -3542,7 +3571,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -3554,13 +3583,13 @@
         <v>16</v>
       </c>
       <c r="E84" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F84">
-        <v>1</v>
+        <v>399</v>
       </c>
       <c r="G84">
-        <v>16</v>
+        <v>414</v>
       </c>
       <c r="H84">
         <v>16</v>
@@ -3571,28 +3600,28 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C85">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D85">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E85" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F85">
-        <v>399</v>
+        <v>58</v>
       </c>
       <c r="G85">
-        <v>414</v>
+        <v>79</v>
       </c>
       <c r="H85">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I85">
         <v>16</v>
@@ -3600,13 +3629,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B86">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C86">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D86">
         <v>10</v>
@@ -3629,28 +3658,28 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="B87">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C87">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D87">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E87" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="F87">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="G87">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H87">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I87">
         <v>16</v>
@@ -3658,28 +3687,28 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="B88">
         <v>1</v>
       </c>
       <c r="C88">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D88">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E88" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="F88">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="G88">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="H88">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I88">
         <v>16</v>
@@ -3687,57 +3716,57 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="C89">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="D89">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E89" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="F89">
-        <v>1</v>
+        <v>324</v>
       </c>
       <c r="G89">
-        <v>16</v>
+        <v>345</v>
       </c>
       <c r="H89">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I89">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="B90">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C90">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="D90">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E90" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="F90">
-        <v>324</v>
+        <v>37</v>
       </c>
       <c r="G90">
-        <v>345</v>
+        <v>55</v>
       </c>
       <c r="H90">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="I90">
         <v>15</v>
@@ -3745,28 +3774,28 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="B91">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C91">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D91">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E91" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="F91">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="G91">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="H91">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I91">
         <v>15</v>
@@ -3774,28 +3803,28 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B92">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C92">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D92">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E92" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="F92">
-        <v>67</v>
+        <v>197</v>
       </c>
       <c r="G92">
-        <v>83</v>
+        <v>215</v>
       </c>
       <c r="H92">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I92">
         <v>15</v>
@@ -3803,25 +3832,25 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>72</v>
+      </c>
+      <c r="C93">
         <v>82</v>
-      </c>
-      <c r="B93">
-        <v>29</v>
-      </c>
-      <c r="C93">
-        <v>39</v>
       </c>
       <c r="D93">
         <v>11</v>
       </c>
       <c r="E93" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F93">
-        <v>197</v>
+        <v>93</v>
       </c>
       <c r="G93">
-        <v>215</v>
+        <v>111</v>
       </c>
       <c r="H93">
         <v>19</v>
@@ -3832,13 +3861,13 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B94">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="C94">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="D94">
         <v>11</v>
@@ -3859,38 +3888,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>112</v>
-      </c>
-      <c r="B95">
-        <v>16</v>
-      </c>
-      <c r="C95">
-        <v>26</v>
-      </c>
-      <c r="D95">
-        <v>11</v>
-      </c>
-      <c r="E95" t="s">
-        <v>92</v>
-      </c>
-      <c r="F95">
-        <v>93</v>
-      </c>
-      <c r="G95">
-        <v>111</v>
-      </c>
-      <c r="H95">
-        <v>19</v>
-      </c>
-      <c r="I95">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A1:J29">
-    <sortCondition descending="1" ref="J1:J29"/>
+  <sortState ref="A1:L95">
+    <sortCondition descending="1" ref="I1:I95"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>